<commit_message>
updating image analysis images
</commit_message>
<xml_diff>
--- a/image analysis examples/BIGMNI03/res.xlsx
+++ b/image analysis examples/BIGMNI03/res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>dendrite id</t>
   </si>
@@ -46,163 +46,151 @@
     <t>distance to parallel [μm]</t>
   </si>
   <si>
-    <t>(x: 0, y: 64)</t>
-  </si>
-  <si>
-    <t>(x: 100, y: 118)</t>
-  </si>
-  <si>
-    <t>(x: 33, y: 14)</t>
-  </si>
-  <si>
-    <t>(x: 96, y: 72)</t>
-  </si>
-  <si>
-    <t>6 , 8</t>
-  </si>
-  <si>
-    <t>11.59 , 0.44</t>
-  </si>
-  <si>
-    <t>(x: 44, y: 201)</t>
-  </si>
-  <si>
-    <t>(x: 105, y: 140)</t>
+    <t>(x: 0, y: 75)</t>
+  </si>
+  <si>
+    <t>(x: 81, y: 108)</t>
+  </si>
+  <si>
+    <t>(x: 5, y: 65)</t>
+  </si>
+  <si>
+    <t>(x: 99, y: 118)</t>
+  </si>
+  <si>
+    <t>(x: 19, y: 6)</t>
+  </si>
+  <si>
+    <t>(x: 107, y: 82)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>17.66</t>
+  </si>
+  <si>
+    <t>(x: 20, y: 161)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>17.26</t>
+  </si>
+  <si>
+    <t>(x: 28, y: 219)</t>
+  </si>
+  <si>
+    <t>(x: 101, y: 149)</t>
+  </si>
+  <si>
+    <t>(x: 37, y: 84)</t>
+  </si>
+  <si>
+    <t>(x: 89, y: 98)</t>
+  </si>
+  <si>
+    <t>(x: 88, y: 233)</t>
+  </si>
+  <si>
+    <t>(x: 154, y: 235)</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>19.23</t>
+  </si>
+  <si>
+    <t>(x: 159, y: 102)</t>
+  </si>
+  <si>
+    <t>(x: 252, y: 31)</t>
+  </si>
+  <si>
+    <t>(x: 159, y: 113)</t>
+  </si>
+  <si>
+    <t>(x: 246, y: 96)</t>
+  </si>
+  <si>
+    <t>(x: 175, y: 163)</t>
+  </si>
+  <si>
+    <t>(x: 254, y: 238)</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>(x: 182, y: 105)</t>
+  </si>
+  <si>
+    <t>(x: 253, y: 103)</t>
+  </si>
+  <si>
+    <t>(x: 190, y: 69)</t>
+  </si>
+  <si>
+    <t>(x: 252, y: 36)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>(x: 199, y: 129)</t>
+  </si>
+  <si>
+    <t>(x: 252, y: 131)</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>14.33</t>
-  </si>
-  <si>
-    <t>(x: 85, y: 235)</t>
-  </si>
-  <si>
-    <t>(x: 166, y: 235)</t>
-  </si>
-  <si>
-    <t>(x: 139, y: 113)</t>
-  </si>
-  <si>
-    <t>(x: 255, y: 96)</t>
-  </si>
-  <si>
-    <t>(x: 142, y: 124)</t>
-  </si>
-  <si>
-    <t>(x: 239, y: 221)</t>
-  </si>
-  <si>
-    <t>2 , 8</t>
-  </si>
-  <si>
-    <t>11.59 , 7.49</t>
-  </si>
-  <si>
-    <t>(x: 174, y: 89)</t>
-  </si>
-  <si>
-    <t>(x: 251, y: 28)</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>(x: 38, y: 0)</t>
-  </si>
-  <si>
-    <t>(x: 114, y: 89)</t>
-  </si>
-  <si>
-    <t>2 , 6 , 9</t>
-  </si>
-  <si>
-    <t>0.44 , 7.49 , 2.69</t>
-  </si>
-  <si>
-    <t>(x: 39, y: 26)</t>
-  </si>
-  <si>
-    <t>(x: 149, y: 211)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>2.69</t>
-  </si>
-  <si>
-    <t>(x: 172, y: 22)</t>
-  </si>
-  <si>
-    <t>(x: 141, y: 115)</t>
-  </si>
-  <si>
-    <t>14 , 13 , 15 , 12</t>
-  </si>
-  <si>
-    <t>10.0 , 11.7 , 16.35 , 18.3</t>
-  </si>
-  <si>
-    <t>(x: 103, y: 137)</t>
-  </si>
-  <si>
-    <t>(x: 101, y: 253)</t>
-  </si>
-  <si>
-    <t>14 , 13</t>
-  </si>
-  <si>
-    <t>2.64 , 4.47</t>
-  </si>
-  <si>
-    <t>(x: 43, y: 164)</t>
-  </si>
-  <si>
-    <t>(x: 17, y: 227)</t>
-  </si>
-  <si>
-    <t>13 , 15 , 10</t>
-  </si>
-  <si>
-    <t>16.25 , 3.01 , 18.3</t>
-  </si>
-  <si>
-    <t>(x: 138, y: 185)</t>
-  </si>
-  <si>
-    <t>(x: 128, y: 238)</t>
-  </si>
-  <si>
-    <t>11 , 14 , 15 , 10 , 12</t>
-  </si>
-  <si>
-    <t>4.47 , 1.72 , 13.26 , 11.7 , 16.25</t>
-  </si>
-  <si>
-    <t>(x: 126, y: 173)</t>
-  </si>
-  <si>
-    <t>(x: 117, y: 243)</t>
-  </si>
-  <si>
-    <t>11 , 13 , 15 , 10</t>
-  </si>
-  <si>
-    <t>2.64 , 1.72 , 11.0 , 10.0</t>
-  </si>
-  <si>
-    <t>(x: 60, y: 170)</t>
-  </si>
-  <si>
-    <t>(x: 37, y: 246)</t>
-  </si>
-  <si>
-    <t>14 , 13 , 10 , 12</t>
-  </si>
-  <si>
-    <t>11.0 , 13.26 , 16.35 , 3.01</t>
+    <t>(x: 39, y: 3)</t>
+  </si>
+  <si>
+    <t>(x: 111, y: 86)</t>
+  </si>
+  <si>
+    <t>(x: 64, y: 40)</t>
+  </si>
+  <si>
+    <t>(x: 100, y: 128)</t>
+  </si>
+  <si>
+    <t>(x: 68, y: 69)</t>
+  </si>
+  <si>
+    <t>(x: 101, y: 121)</t>
+  </si>
+  <si>
+    <t>(x: 173, y: 1)</t>
+  </si>
+  <si>
+    <t>(x: 140, y: 84)</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>18.48</t>
+  </si>
+  <si>
+    <t>(x: 49, y: 147)</t>
+  </si>
+  <si>
+    <t>(x: 23, y: 211)</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>(x: 129, y: 149)</t>
+  </si>
+  <si>
+    <t>(x: 120, y: 217)</t>
   </si>
 </sst>
 </file>
@@ -534,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -577,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>18.98</v>
+        <v>14.61</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -586,13 +574,13 @@
         <v>11</v>
       </c>
       <c r="E2">
-        <v>28.37</v>
+        <v>22.17</v>
       </c>
       <c r="F2">
-        <v>16.37</v>
+        <v>17.17</v>
       </c>
       <c r="G2">
-        <v>40.37</v>
+        <v>27.17</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -603,7 +591,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>14.3</v>
+        <v>18.02</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -612,22 +600,16 @@
         <v>13</v>
       </c>
       <c r="E3">
-        <v>42.63</v>
+        <v>29.42</v>
       </c>
       <c r="F3">
-        <v>30.63</v>
+        <v>24.42</v>
       </c>
       <c r="G3">
-        <v>54.63</v>
+        <v>34.42</v>
       </c>
       <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -635,31 +617,31 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>14.41</v>
+        <v>19.42</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>135</v>
+        <v>40.82</v>
       </c>
       <c r="F4">
-        <v>123</v>
+        <v>35.82</v>
       </c>
       <c r="G4">
-        <v>147</v>
+        <v>45.82</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -667,25 +649,31 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>13.53</v>
+        <v>15.02</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>151.44</v>
+      </c>
+      <c r="F5">
+        <v>146.44</v>
+      </c>
+      <c r="G5">
+        <v>156.44</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>-12</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -693,22 +681,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>19.58</v>
+        <v>16.89</v>
       </c>
       <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
       <c r="E6">
-        <v>171.66</v>
+        <v>136.2</v>
       </c>
       <c r="F6">
-        <v>159.66</v>
+        <v>131.2</v>
       </c>
       <c r="G6">
-        <v>183.66</v>
+        <v>141.2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -719,31 +707,25 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>22.91</v>
+        <v>8.99</v>
       </c>
       <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
       <c r="E7">
-        <v>45</v>
+        <v>15.07</v>
       </c>
       <c r="F7">
-        <v>33</v>
+        <v>10.07</v>
       </c>
       <c r="G7">
-        <v>57</v>
+        <v>20.07</v>
       </c>
       <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -751,31 +733,31 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>16.41</v>
+        <v>11.03</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8">
-        <v>141.61</v>
+        <v>1.74</v>
       </c>
       <c r="F8">
-        <v>129.61</v>
+        <v>-3.26</v>
       </c>
       <c r="G8">
-        <v>153.61</v>
+        <v>6.74</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -786,28 +768,22 @@
         <v>19.54</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>49.5</v>
+        <v>142.64</v>
       </c>
       <c r="F9">
-        <v>37.5</v>
+        <v>137.64</v>
       </c>
       <c r="G9">
-        <v>61.5</v>
+        <v>147.64</v>
       </c>
       <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -815,31 +791,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>35.94</v>
+        <v>14.8</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E10">
-        <v>59.26</v>
+        <v>168.94</v>
       </c>
       <c r="F10">
-        <v>47.26</v>
+        <v>163.94</v>
       </c>
       <c r="G10">
-        <v>71.26000000000001</v>
+        <v>173.94</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -847,31 +817,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>16.37</v>
+        <v>18.19</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E11">
-        <v>108.43</v>
+        <v>43.51</v>
       </c>
       <c r="F11">
-        <v>96.43000000000001</v>
+        <v>38.51</v>
       </c>
       <c r="G11">
-        <v>120.43</v>
+        <v>48.51</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -879,31 +849,25 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>19.37</v>
+        <v>11.86</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>90.98999999999999</v>
+        <v>178.39</v>
       </c>
       <c r="F12">
-        <v>78.98999999999999</v>
+        <v>173.39</v>
       </c>
       <c r="G12">
-        <v>102.99</v>
+        <v>183.39</v>
       </c>
       <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -911,31 +875,31 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>11.38</v>
+        <v>11.73</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E13">
-        <v>112.43</v>
+        <v>151.98</v>
       </c>
       <c r="F13">
-        <v>100.43</v>
+        <v>146.98</v>
       </c>
       <c r="G13">
-        <v>124.43</v>
+        <v>156.98</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -943,31 +907,31 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>9.01</v>
+        <v>8.859999999999999</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E14">
-        <v>100.68</v>
+        <v>2.16</v>
       </c>
       <c r="F14">
-        <v>88.68000000000001</v>
+        <v>-2.84</v>
       </c>
       <c r="G14">
-        <v>112.68</v>
+        <v>7.16</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -975,31 +939,25 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>11.79</v>
+        <v>18.35</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E15">
-        <v>97.33</v>
+        <v>49.06</v>
       </c>
       <c r="F15">
-        <v>85.33</v>
+        <v>44.06</v>
       </c>
       <c r="G15">
-        <v>109.33</v>
+        <v>54.06</v>
       </c>
       <c r="H15">
-        <v>4</v>
-      </c>
-      <c r="I15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1007,31 +965,141 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>13.26</v>
+        <v>15.88</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E16">
-        <v>106.84</v>
+        <v>67.75</v>
       </c>
       <c r="F16">
-        <v>94.84</v>
+        <v>62.75</v>
       </c>
       <c r="G16">
-        <v>118.84</v>
+        <v>72.75</v>
       </c>
       <c r="H16">
-        <v>4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" t="s">
-        <v>62</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>10.29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17">
+        <v>57.6</v>
+      </c>
+      <c r="F17">
+        <v>52.6</v>
+      </c>
+      <c r="G17">
+        <v>62.6</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>14.92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18">
+        <v>111.68</v>
+      </c>
+      <c r="F18">
+        <v>106.68</v>
+      </c>
+      <c r="G18">
+        <v>116.68</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>11.54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19">
+        <v>112.11</v>
+      </c>
+      <c r="F19">
+        <v>107.11</v>
+      </c>
+      <c r="G19">
+        <v>117.11</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>11.46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20">
+        <v>97.54000000000001</v>
+      </c>
+      <c r="F20">
+        <v>92.54000000000001</v>
+      </c>
+      <c r="G20">
+        <v>102.54</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>